<commit_message>
Updated with already solved exercises
</commit_message>
<xml_diff>
--- a/chapter1/Chapter1-1a.xlsx
+++ b/chapter1/Chapter1-1a.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hong\booksWriting\dataMiningInExcel\Chapter1\examples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FC3347-890E-4569-B601-314C0E92873D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="990" windowWidth="11610" windowHeight="8445" xr2:uid="{99981357-CC79-459C-B8F1-C394E398F6CE}"/>
+    <workbookView xWindow="4872" yWindow="996" windowWidth="11616" windowHeight="8448"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -60,11 +54,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,7 +90,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -209,7 +203,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -403,26 +397,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6729E8-5BD1-48F1-859E-9DE564D871C9}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -446,9 +438,13 @@
       <c r="C2" s="2">
         <v>50500</v>
       </c>
+      <c r="D2">
+        <f>IF(C2&lt;=50000,0,IF(C2&lt;=100000,(C2-50000)*10%,50000*0.1+(C2-100000)*20%))</f>
+        <v>50</v>
+      </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -458,8 +454,12 @@
       <c r="C3" s="2">
         <v>100200</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">IF(C3&lt;=50000,0,IF(C3&lt;=100000,(C3-50000)*10%,50000*0.1+(C3-100000)*20%))</f>
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -469,8 +469,12 @@
       <c r="C4" s="2">
         <v>86000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -480,8 +484,12 @@
       <c r="C5" s="2">
         <v>120000</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -491,8 +499,12 @@
       <c r="C6" s="2">
         <v>87000</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -502,8 +514,12 @@
       <c r="C7" s="2">
         <v>98000</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -513,8 +529,12 @@
       <c r="C8" s="2">
         <v>75000</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -524,8 +544,12 @@
       <c r="C9" s="2">
         <v>110000</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -535,9 +559,19 @@
       <c r="C10" s="2">
         <v>88000</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13">
+        <f>COUNTIFS(B2:B10,1,C2:C10,"&gt;50000",C2:C10,"&lt;=100000")</f>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A10">
+  <sortState ref="A2:A10">
     <sortCondition ref="A2:A10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>